<commit_message>
Data used for plots
</commit_message>
<xml_diff>
--- a/Shor_Data.xlsx
+++ b/Shor_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geige\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tumde-my.sharepoint.com/personal/laura9_geiger_tum_de/Documents/Dokumente/5 TUM/24WS/DD2367 Quantum Computing/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD7927-844C-44E8-8308-E2249140C009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{900C2FDF-6761-408E-8ECA-87D02B84A7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9706236-D419-4A17-AFF4-BBBCD403CF6C}"/>
   <bookViews>
     <workbookView xWindow="1163" yWindow="-98" windowWidth="19454" windowHeight="13875" xr2:uid="{8599C618-5A94-A04D-AC03-F3C749859BA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="90">
   <si>
     <t>Algorithm</t>
   </si>
@@ -126,31 +126,19 @@
     <t>c7</t>
   </si>
   <si>
-    <t>1 m 6s</t>
-  </si>
-  <si>
     <t>cwr8kyz2ac5g008hxaqg</t>
   </si>
   <si>
     <t>c8</t>
   </si>
   <si>
-    <t>1m 6s</t>
-  </si>
-  <si>
     <t>cwrt51c997wg008xg020</t>
   </si>
   <si>
     <t>cwrxh14tdtng0086yr5g</t>
   </si>
   <si>
-    <t xml:space="preserve">1m 30s </t>
-  </si>
-  <si>
     <t>cwryb4ctdtng0086ys8g</t>
-  </si>
-  <si>
-    <t>1m 29s</t>
   </si>
   <si>
     <t>cwrztrvehebg008j1k1g</t>
@@ -328,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +329,13 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -387,19 +382,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,17 +707,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F36CD9-68E0-A24E-B94C-DEFAD14B9FAF}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="5" max="5" width="16.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="11" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
@@ -744,7 +740,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -782,7 +778,7 @@
       <c r="F2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>0.546875</v>
       </c>
       <c r="H2">
@@ -811,7 +807,7 @@
       <c r="F3">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>0.53906200000000004</v>
       </c>
       <c r="H3">
@@ -840,7 +836,7 @@
       <c r="F4">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>0.296875</v>
       </c>
       <c r="H4">
@@ -866,7 +862,7 @@
       <c r="E5">
         <v>49.794899999999998</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5">
@@ -889,7 +885,7 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
       <c r="H6">
@@ -918,7 +914,7 @@
       <c r="F7">
         <v>1E-4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>0.453125</v>
       </c>
       <c r="H7">
@@ -944,7 +940,7 @@
       <c r="E8">
         <v>333.45440000000002</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -964,7 +960,7 @@
       <c r="E9">
         <v>2176.4168</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>0.39843800000000001</v>
       </c>
     </row>
@@ -984,7 +980,7 @@
       <c r="E10">
         <v>1524.155</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="4">
         <v>0.53125</v>
       </c>
     </row>
@@ -1004,7 +1000,7 @@
       <c r="E11">
         <v>339.04270000000002</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>0.140625</v>
       </c>
     </row>
@@ -1024,7 +1020,7 @@
       <c r="E12">
         <v>1386.4290000000001</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1044,7 +1040,7 @@
       <c r="E13">
         <v>1655.6668</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>0.42968800000000001</v>
       </c>
     </row>
@@ -1064,7 +1060,7 @@
       <c r="E14">
         <v>331.38389999999998</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="4">
         <v>0.296875</v>
       </c>
     </row>
@@ -1084,7 +1080,7 @@
       <c r="E15">
         <v>334.21249999999998</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>7.8125E-2</v>
       </c>
     </row>
@@ -1101,7 +1097,7 @@
       <c r="D16">
         <v>2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1124,7 +1120,7 @@
       <c r="F17">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="4">
         <v>0.24218799999999999</v>
       </c>
       <c r="K17" t="s">
@@ -1153,7 +1149,7 @@
       <c r="F18">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="4">
         <v>0.60156200000000004</v>
       </c>
       <c r="K18" t="s">
@@ -1182,7 +1178,7 @@
       <c r="F19">
         <v>5.3E-3</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="4">
         <v>7.8125E-2</v>
       </c>
       <c r="K19" t="s">
@@ -1211,7 +1207,7 @@
       <c r="F20">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="4">
         <v>0</v>
       </c>
       <c r="H20">
@@ -1243,7 +1239,7 @@
       <c r="E21">
         <v>14</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="4">
         <v>0.109375</v>
       </c>
       <c r="H21">
@@ -1272,7 +1268,7 @@
       <c r="F22">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="4">
         <v>3.125E-2</v>
       </c>
       <c r="H22">
@@ -1304,7 +1300,7 @@
       <c r="E23">
         <v>14</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="4">
         <v>0.50781200000000004</v>
       </c>
       <c r="H23">
@@ -1330,7 +1326,7 @@
       <c r="E24">
         <v>14</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="4">
         <v>3.125E-2</v>
       </c>
       <c r="H24">
@@ -1356,7 +1352,7 @@
       <c r="E25">
         <v>14</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="4">
         <v>4.6875E-2</v>
       </c>
       <c r="H25">
@@ -1385,7 +1381,7 @@
       <c r="F26">
         <v>4.3E-3</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="4">
         <v>1.5625E-2</v>
       </c>
       <c r="H26">
@@ -1417,7 +1413,7 @@
       <c r="E27">
         <v>14</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="4">
         <v>1.5625E-2</v>
       </c>
       <c r="H27">
@@ -1443,7 +1439,7 @@
       <c r="E28">
         <v>24</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="4">
         <v>2.3438000000000001E-2</v>
       </c>
       <c r="H28">
@@ -1469,7 +1465,7 @@
       <c r="E29">
         <v>24</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="4">
         <v>0</v>
       </c>
       <c r="H29">
@@ -1495,7 +1491,7 @@
       <c r="E30">
         <v>24</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="4">
         <v>0</v>
       </c>
       <c r="H30">
@@ -1521,7 +1517,7 @@
       <c r="E31">
         <v>24</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="4">
         <v>3.9061999999999999E-2</v>
       </c>
       <c r="H31">
@@ -1547,7 +1543,7 @@
       <c r="E32">
         <v>24</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="4">
         <v>1.5625E-2</v>
       </c>
       <c r="H32">
@@ -1573,7 +1569,7 @@
       <c r="E33">
         <v>29</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="4">
         <v>0</v>
       </c>
       <c r="H33">
@@ -1599,7 +1595,7 @@
       <c r="E34">
         <v>50</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="4">
         <v>9.375E-2</v>
       </c>
       <c r="H34">
@@ -1628,7 +1624,7 @@
       <c r="F35">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="4">
         <v>2.3438000000000001E-2</v>
       </c>
       <c r="H35">
@@ -1657,13 +1653,13 @@
       <c r="D36">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
-        <v>29</v>
+      <c r="E36">
+        <v>66</v>
       </c>
       <c r="F36">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="4">
         <v>0</v>
       </c>
       <c r="H36">
@@ -1673,10 +1669,10 @@
         <v>42</v>
       </c>
       <c r="K36" t="s">
+        <v>29</v>
+      </c>
+      <c r="L36" t="s">
         <v>30</v>
-      </c>
-      <c r="L36" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.5">
@@ -1692,6 +1688,27 @@
       <c r="D37">
         <v>2</v>
       </c>
+      <c r="E37">
+        <v>67</v>
+      </c>
+      <c r="F37">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>322905</v>
+      </c>
+      <c r="I37">
+        <v>42</v>
+      </c>
+      <c r="K37" t="s">
+        <v>29</v>
+      </c>
+      <c r="L37" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
@@ -1706,13 +1723,13 @@
       <c r="D38">
         <v>2</v>
       </c>
-      <c r="E38" t="s">
-        <v>32</v>
+      <c r="E38">
+        <v>66</v>
       </c>
       <c r="F38">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="4">
         <v>0</v>
       </c>
       <c r="H38">
@@ -1722,7 +1739,7 @@
         <v>42</v>
       </c>
       <c r="K38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L38" t="s">
         <v>26</v>
@@ -1741,13 +1758,13 @@
       <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" t="s">
-        <v>32</v>
+      <c r="E39">
+        <v>66</v>
       </c>
       <c r="F39">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="4">
         <v>0</v>
       </c>
       <c r="H39">
@@ -1757,7 +1774,7 @@
         <v>42</v>
       </c>
       <c r="K39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L39" t="s">
         <v>24</v>
@@ -1776,13 +1793,13 @@
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
-        <v>35</v>
+      <c r="E40">
+        <v>90</v>
       </c>
       <c r="F40">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="4">
         <v>0</v>
       </c>
       <c r="H40">
@@ -1792,7 +1809,7 @@
         <v>46</v>
       </c>
       <c r="K40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L40" t="s">
         <v>22</v>
@@ -1811,8 +1828,11 @@
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
-        <v>37</v>
+      <c r="E41">
+        <v>89</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
       </c>
       <c r="H41">
         <v>446761</v>
@@ -1821,7 +1841,7 @@
         <v>46</v>
       </c>
       <c r="K41" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L41" t="s">
         <v>20</v>
@@ -1829,101 +1849,185 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>1263</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>2</v>
+      </c>
+      <c r="E42">
+        <v>0.1041</v>
+      </c>
+      <c r="F42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.796875</v>
+      </c>
+      <c r="H42">
+        <v>418</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43">
-        <v>1363</v>
+        <v>21</v>
       </c>
       <c r="D43">
         <v>2</v>
+      </c>
+      <c r="E43">
+        <v>0.15920000000000001</v>
+      </c>
+      <c r="F43">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.703125</v>
+      </c>
+      <c r="H43">
+        <v>852</v>
+      </c>
+      <c r="I43">
+        <v>12</v>
+      </c>
+      <c r="J43">
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>1469</v>
+        <v>33</v>
       </c>
       <c r="D44">
         <v>2</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1530</v>
+      </c>
+      <c r="I44">
+        <v>14</v>
+      </c>
+      <c r="J44">
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <v>1589</v>
+        <v>35</v>
       </c>
       <c r="D45">
         <v>2</v>
+      </c>
+      <c r="E45">
+        <v>0.70530000000000004</v>
+      </c>
+      <c r="F45">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.6796875</v>
+      </c>
+      <c r="H45">
+        <v>2226</v>
+      </c>
+      <c r="I45">
+        <v>14</v>
+      </c>
+      <c r="J45">
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>1703</v>
+        <v>39</v>
       </c>
       <c r="D46">
         <v>2</v>
+      </c>
+      <c r="E46">
+        <v>0.36880000000000002</v>
+      </c>
+      <c r="F46">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.6796875</v>
+      </c>
+      <c r="H46">
+        <v>2806</v>
+      </c>
+      <c r="I46">
+        <v>14</v>
+      </c>
+      <c r="J46">
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
       </c>
       <c r="C47">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0.1041</v>
+        <v>0.2712</v>
       </c>
       <c r="F47">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0.796875</v>
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.890625</v>
       </c>
       <c r="H47">
-        <v>418</v>
+        <v>2574</v>
       </c>
       <c r="I47">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J47">
         <v>128</v>
@@ -1931,31 +2035,31 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
       </c>
       <c r="C48">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48">
-        <v>0.15920000000000001</v>
+        <v>0.52769999999999995</v>
       </c>
       <c r="F48">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="G48" s="3">
-        <v>0.703125</v>
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.328125</v>
       </c>
       <c r="H48">
-        <v>852</v>
+        <v>3154</v>
       </c>
       <c r="I48">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J48">
         <v>128</v>
@@ -1963,25 +2067,31 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
       <c r="C49">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
-      <c r="G49" s="1">
-        <v>0</v>
+      <c r="E49">
+        <v>0.59819999999999995</v>
+      </c>
+      <c r="F49">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.4765625</v>
       </c>
       <c r="H49">
-        <v>1530</v>
+        <v>4992</v>
       </c>
       <c r="I49">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J49">
         <v>128</v>
@@ -1989,31 +2099,31 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
       </c>
       <c r="C50">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50">
-        <v>0.70530000000000004</v>
+        <v>0.52990000000000004</v>
       </c>
       <c r="F50">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0.6796875</v>
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0.890625</v>
       </c>
       <c r="H50">
-        <v>2226</v>
+        <v>7170</v>
       </c>
       <c r="I50">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J50">
         <v>128</v>
@@ -2021,31 +2131,31 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
       </c>
       <c r="C51">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51">
-        <v>0.36880000000000002</v>
+        <v>1.1820999999999999</v>
       </c>
       <c r="F51">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0.6796875</v>
+        <v>1.06E-2</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0.5390625</v>
       </c>
       <c r="H51">
-        <v>2806</v>
+        <v>8380</v>
       </c>
       <c r="I51">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J51">
         <v>128</v>
@@ -2053,31 +2163,31 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
         <v>13</v>
       </c>
       <c r="C52">
-        <v>51</v>
+        <v>203</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52">
-        <v>0.2712</v>
+        <v>0.85560000000000003</v>
       </c>
       <c r="F52">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="G52" s="2">
-        <v>0.890625</v>
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="G52" s="4">
+        <v>0.15625</v>
       </c>
       <c r="H52">
-        <v>2574</v>
+        <v>16405</v>
       </c>
       <c r="I52">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J52">
         <v>128</v>
@@ -2085,695 +2195,695 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53">
-        <v>0.52769999999999995</v>
+        <v>4</v>
       </c>
       <c r="F53">
-        <v>1.6299999999999999E-2</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0.328125</v>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G53" s="4">
+        <v>0.2421875</v>
       </c>
       <c r="H53">
-        <v>3154</v>
+        <v>418</v>
       </c>
       <c r="I53">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J53">
         <v>128</v>
+      </c>
+      <c r="K53" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
       <c r="E54">
-        <v>0.59819999999999995</v>
+        <v>10</v>
       </c>
       <c r="F54">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0.4765625</v>
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.40625</v>
       </c>
       <c r="H54">
-        <v>4992</v>
+        <v>852</v>
       </c>
       <c r="I54">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J54">
         <v>128</v>
+      </c>
+      <c r="K54" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C55">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55">
-        <v>0.52990000000000004</v>
-      </c>
-      <c r="F55">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0.890625</v>
+        <v>27</v>
+      </c>
+      <c r="G55" s="4">
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>7170</v>
+        <v>1530</v>
       </c>
       <c r="I55">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J55">
         <v>128</v>
+      </c>
+      <c r="K55" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>35</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>38</v>
+      </c>
+      <c r="F56">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.2421875</v>
+      </c>
+      <c r="H56">
+        <v>2226</v>
+      </c>
+      <c r="I56">
+        <v>14</v>
+      </c>
+      <c r="J56">
+        <v>128</v>
+      </c>
+      <c r="K56" t="s">
         <v>39</v>
-      </c>
-      <c r="B56" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56">
-        <v>119</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
-      </c>
-      <c r="E56">
-        <v>1.1820999999999999</v>
-      </c>
-      <c r="F56">
-        <v>1.06E-2</v>
-      </c>
-      <c r="G56" s="2">
-        <v>0.5390625</v>
-      </c>
-      <c r="H56">
-        <v>8380</v>
-      </c>
-      <c r="I56">
-        <v>16</v>
-      </c>
-      <c r="J56">
-        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
         <v>39</v>
       </c>
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57">
-        <v>203</v>
-      </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57">
-        <v>0.85560000000000003</v>
+        <v>44</v>
       </c>
       <c r="F57">
-        <v>1.6899999999999998E-2</v>
-      </c>
-      <c r="G57" s="2">
-        <v>0.15625</v>
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0.28125</v>
       </c>
       <c r="H57">
-        <v>16405</v>
+        <v>2806</v>
       </c>
       <c r="I57">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J57">
         <v>128</v>
+      </c>
+      <c r="K57" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F58">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="G58" s="2">
-        <v>0.2421875</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G58" s="4">
+        <v>7.8125E-2</v>
       </c>
       <c r="H58">
-        <v>418</v>
+        <v>3154</v>
       </c>
       <c r="I58">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J58">
         <v>128</v>
       </c>
       <c r="K58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
         <v>14</v>
       </c>
       <c r="C59">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D59">
         <v>2</v>
       </c>
       <c r="E59">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="F59">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="G59" s="2">
-        <v>0.40625</v>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0.1640625</v>
       </c>
       <c r="H59">
-        <v>852</v>
+        <v>4992</v>
       </c>
       <c r="I59">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J59">
         <v>128</v>
       </c>
       <c r="K59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B60" t="s">
         <v>14</v>
       </c>
       <c r="C60">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
       <c r="E60">
-        <v>27</v>
-      </c>
-      <c r="G60" s="1">
-        <v>0</v>
+        <v>116</v>
+      </c>
+      <c r="F60">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="G60" s="4">
+        <v>0.1953125</v>
       </c>
       <c r="H60">
-        <v>1530</v>
+        <v>6202</v>
       </c>
       <c r="I60">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J60">
         <v>128</v>
       </c>
       <c r="K60" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
         <v>14</v>
       </c>
       <c r="C61">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="F61">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.2421875</v>
+        <v>1.46E-2</v>
+      </c>
+      <c r="G61" s="4">
+        <v>0.28125</v>
       </c>
       <c r="H61">
-        <v>2226</v>
+        <v>5960</v>
       </c>
       <c r="I61">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J61">
         <v>128</v>
       </c>
       <c r="K61" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
         <v>14</v>
       </c>
       <c r="C62">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="F62">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="G62" s="2">
-        <v>0.28125</v>
+        <v>6.6E-3</v>
+      </c>
+      <c r="G62" s="4">
+        <v>0.359375</v>
       </c>
       <c r="H62">
-        <v>2806</v>
+        <v>7170</v>
       </c>
       <c r="I62">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J62">
         <v>128</v>
       </c>
       <c r="K62" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
         <v>14</v>
       </c>
       <c r="C63">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63">
+        <v>150</v>
+      </c>
+      <c r="F63">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0.1484375</v>
+      </c>
+      <c r="H63">
+        <v>8380</v>
+      </c>
+      <c r="I63">
+        <v>16</v>
+      </c>
+      <c r="J63">
+        <v>128</v>
+      </c>
+      <c r="K63" t="s">
         <v>46</v>
-      </c>
-      <c r="F63">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G63" s="2">
-        <v>7.8125E-2</v>
-      </c>
-      <c r="H63">
-        <v>3154</v>
-      </c>
-      <c r="I63">
-        <v>14</v>
-      </c>
-      <c r="J63">
-        <v>128</v>
-      </c>
-      <c r="K63" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>14</v>
       </c>
       <c r="C64">
-        <v>69</v>
+        <v>203</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
-      <c r="E64">
-        <v>107</v>
-      </c>
-      <c r="F64">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0.1640625</v>
+      <c r="G64" s="4">
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>4992</v>
+        <v>16405</v>
       </c>
       <c r="I64">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J64">
         <v>128</v>
       </c>
       <c r="K64" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65">
-        <v>116</v>
+        <v>1.18474960327148E-2</v>
       </c>
       <c r="F65">
-        <v>8.0999999999999996E-3</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0.1953125</v>
+        <v>1.0523796081542899E-2</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0.27500000000000002</v>
       </c>
       <c r="H65">
-        <v>6202</v>
+        <v>17275</v>
       </c>
       <c r="I65">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J65">
         <v>128</v>
       </c>
-      <c r="K65" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
       <c r="E66">
-        <v>115</v>
+        <v>1.1539459228515601E-4</v>
       </c>
       <c r="F66">
-        <v>1.46E-2</v>
-      </c>
-      <c r="G66" s="2">
-        <v>0.28125</v>
+        <v>9.5095634460449201E-3</v>
+      </c>
+      <c r="G66" s="4">
+        <v>0.23728813559322001</v>
       </c>
       <c r="H66">
-        <v>5960</v>
+        <v>32912</v>
       </c>
       <c r="I66">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="J66">
         <v>128</v>
       </c>
-      <c r="K66" t="s">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A67" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A67" t="s">
-        <v>39</v>
-      </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C67">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67">
-        <v>117</v>
+        <v>1.1467933654785099E-4</v>
       </c>
       <c r="F67">
-        <v>6.6E-3</v>
-      </c>
-      <c r="G67" s="2">
-        <v>0.359375</v>
+        <v>3.70151996612548E-2</v>
+      </c>
+      <c r="G67" s="4">
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>7170</v>
+        <v>56384</v>
       </c>
       <c r="I67">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J67">
         <v>128</v>
       </c>
-      <c r="K67" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C68">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
       <c r="E68">
-        <v>150</v>
+        <v>1.3899803161620999E-4</v>
       </c>
       <c r="F68">
-        <v>6.6E-3</v>
-      </c>
-      <c r="G68" s="2">
-        <v>0.1484375</v>
+        <v>4.1440725326538003E-2</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0.180722891566265</v>
       </c>
       <c r="H68">
-        <v>8380</v>
+        <v>56516</v>
       </c>
       <c r="I68">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J68">
         <v>128</v>
       </c>
-      <c r="K68" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C69">
-        <v>203</v>
+        <v>51</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
-      <c r="G69" s="1">
-        <v>0</v>
+      <c r="E69">
+        <v>1.3446807861328101E-4</v>
+      </c>
+      <c r="F69">
+        <v>1.6571044921875E-2</v>
+      </c>
+      <c r="G69" s="4">
+        <v>0.18333333333333299</v>
       </c>
       <c r="H69">
-        <v>16405</v>
+        <v>54973</v>
       </c>
       <c r="I69">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="J69">
         <v>128</v>
       </c>
-      <c r="K69" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
         <v>13</v>
       </c>
       <c r="C70">
+        <v>55</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>1.0776519775390601E-4</v>
+      </c>
+      <c r="F70">
+        <v>4.9282550811767502E-2</v>
+      </c>
+      <c r="G70" s="4">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="H70">
+        <v>56512</v>
+      </c>
+      <c r="I70">
+        <v>26</v>
+      </c>
+      <c r="J70">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
         <v>15</v>
       </c>
-      <c r="D70">
-        <v>2</v>
-      </c>
-      <c r="E70">
-        <v>1.18474960327148E-2</v>
-      </c>
-      <c r="F70">
-        <v>1.0523796081542899E-2</v>
-      </c>
-      <c r="G70">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="H70">
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>10</v>
+      </c>
+      <c r="F71">
+        <v>9.5086097717285104E-3</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0.2734375</v>
+      </c>
+      <c r="H71">
         <v>17275</v>
       </c>
-      <c r="I70">
+      <c r="I71">
         <v>18</v>
       </c>
-      <c r="J70">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A71" t="s">
-        <v>52</v>
-      </c>
-      <c r="B71" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71">
+      <c r="J71">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A72" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
         <v>21</v>
       </c>
-      <c r="D71">
-        <v>2</v>
-      </c>
-      <c r="E71">
-        <v>1.1539459228515601E-4</v>
-      </c>
-      <c r="F71">
-        <v>9.5095634460449201E-3</v>
-      </c>
-      <c r="G71">
-        <v>0.23728813559322001</v>
-      </c>
-      <c r="H71">
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>10</v>
+      </c>
+      <c r="F72">
+        <v>9.2699527740478498E-3</v>
+      </c>
+      <c r="G72" s="4">
+        <v>0.16521739130434701</v>
+      </c>
+      <c r="H72">
         <v>32912</v>
       </c>
-      <c r="I71">
+      <c r="I72">
         <v>22</v>
       </c>
-      <c r="J71">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A72" t="s">
-        <v>52</v>
-      </c>
-      <c r="B72" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72">
+      <c r="J72">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
         <v>33</v>
       </c>
-      <c r="D72">
-        <v>2</v>
-      </c>
-      <c r="E72">
-        <v>1.1467933654785099E-4</v>
-      </c>
-      <c r="F72">
-        <v>3.70151996612548E-2</v>
-      </c>
-      <c r="G72">
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>15</v>
+      </c>
+      <c r="F73">
+        <v>1.85952186584472E-2</v>
+      </c>
+      <c r="G73" s="4">
         <v>0</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <v>56384</v>
-      </c>
-      <c r="I72">
-        <v>26</v>
-      </c>
-      <c r="J72">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73">
-        <v>35</v>
-      </c>
-      <c r="D73">
-        <v>2</v>
-      </c>
-      <c r="E73">
-        <v>1.3899803161620999E-4</v>
-      </c>
-      <c r="F73">
-        <v>4.1440725326538003E-2</v>
-      </c>
-      <c r="G73">
-        <v>0.180722891566265</v>
-      </c>
-      <c r="H73">
-        <v>56516</v>
       </c>
       <c r="I73">
         <v>26</v>
@@ -2782,30 +2892,30 @@
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D74">
         <v>2</v>
       </c>
       <c r="E74">
-        <v>1.3446807861328101E-4</v>
+        <v>15</v>
       </c>
       <c r="F74">
-        <v>1.6571044921875E-2</v>
-      </c>
-      <c r="G74">
-        <v>0.18333333333333299</v>
+        <v>1.80227756500244E-2</v>
+      </c>
+      <c r="G74" s="4">
+        <v>3.9370078740157403E-2</v>
       </c>
       <c r="H74">
-        <v>54973</v>
+        <v>56516</v>
       </c>
       <c r="I74">
         <v>26</v>
@@ -2814,30 +2924,30 @@
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D75">
         <v>2</v>
       </c>
       <c r="E75">
-        <v>1.0776519775390601E-4</v>
+        <v>15</v>
       </c>
       <c r="F75">
-        <v>4.9282550811767502E-2</v>
-      </c>
-      <c r="G75">
-        <v>7.1428571428571397E-2</v>
+        <v>2.7544021606445299E-2</v>
+      </c>
+      <c r="G75" s="4">
+        <v>7.03125E-2</v>
       </c>
       <c r="H75">
-        <v>56512</v>
+        <v>54973</v>
       </c>
       <c r="I75">
         <v>26</v>
@@ -2846,161 +2956,161 @@
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
       </c>
       <c r="C76">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D76">
         <v>2</v>
       </c>
       <c r="E76">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F76">
-        <v>9.5086097717285104E-3</v>
-      </c>
-      <c r="G76">
-        <v>0.2734375</v>
+        <v>2.6019811630248999E-2</v>
+      </c>
+      <c r="G76" s="4">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H76">
-        <v>17275</v>
+        <v>56512</v>
       </c>
       <c r="I76">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="J76">
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
         <v>14</v>
       </c>
       <c r="C77">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D77">
         <v>2</v>
       </c>
       <c r="E77">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F77">
-        <v>9.2699527740478498E-3</v>
-      </c>
-      <c r="G77">
-        <v>0.16521739130434701</v>
+        <v>3.5067558288574198E-2</v>
+      </c>
+      <c r="G77" s="4">
+        <v>7.9365079365079309E-3</v>
       </c>
       <c r="H77">
-        <v>32912</v>
+        <v>88645</v>
       </c>
       <c r="I77">
+        <v>30</v>
+      </c>
+      <c r="J77">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78">
+        <v>93</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
         <v>22</v>
       </c>
-      <c r="J77">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A78" t="s">
-        <v>52</v>
-      </c>
-      <c r="B78" t="s">
-        <v>14</v>
-      </c>
-      <c r="C78">
-        <v>33</v>
-      </c>
-      <c r="D78">
-        <v>2</v>
-      </c>
-      <c r="E78">
-        <v>15</v>
-      </c>
       <c r="F78">
-        <v>1.85952186584472E-2</v>
-      </c>
-      <c r="G78">
+        <v>5.2066802978515597E-2</v>
+      </c>
+      <c r="G78" s="4">
+        <v>5.5118110236220402E-2</v>
+      </c>
+      <c r="H78">
+        <v>87028</v>
+      </c>
+      <c r="I78">
+        <v>30</v>
+      </c>
+      <c r="J78">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A79" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79">
+        <v>119</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>20</v>
+      </c>
+      <c r="F79">
+        <v>7.6587200164794894E-2</v>
+      </c>
+      <c r="G79" s="4">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H79">
+        <v>88724</v>
+      </c>
+      <c r="I79">
+        <v>30</v>
+      </c>
+      <c r="J79">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80">
+        <v>203</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>31</v>
+      </c>
+      <c r="F80">
+        <v>0.21200394630432101</v>
+      </c>
+      <c r="G80" s="4">
         <v>0</v>
       </c>
-      <c r="H78">
-        <v>56384</v>
-      </c>
-      <c r="I78">
-        <v>26</v>
-      </c>
-      <c r="J78">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A79" t="s">
-        <v>52</v>
-      </c>
-      <c r="B79" t="s">
-        <v>14</v>
-      </c>
-      <c r="C79">
-        <v>35</v>
-      </c>
-      <c r="D79">
-        <v>2</v>
-      </c>
-      <c r="E79">
-        <v>15</v>
-      </c>
-      <c r="F79">
-        <v>1.80227756500244E-2</v>
-      </c>
-      <c r="G79">
-        <v>3.9370078740157403E-2</v>
-      </c>
-      <c r="H79">
-        <v>56516</v>
-      </c>
-      <c r="I79">
-        <v>26</v>
-      </c>
-      <c r="J79">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A80" t="s">
-        <v>52</v>
-      </c>
-      <c r="B80" t="s">
-        <v>14</v>
-      </c>
-      <c r="C80">
-        <v>51</v>
-      </c>
-      <c r="D80">
-        <v>2</v>
-      </c>
-      <c r="E80">
-        <v>15</v>
-      </c>
-      <c r="F80">
-        <v>2.7544021606445299E-2</v>
-      </c>
-      <c r="G80">
-        <v>7.03125E-2</v>
-      </c>
       <c r="H80">
-        <v>54973</v>
+        <v>131034</v>
       </c>
       <c r="I80">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J80">
         <v>128</v>
@@ -3008,31 +3118,31 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B81" t="s">
         <v>14</v>
       </c>
       <c r="C81">
-        <v>55</v>
+        <v>341</v>
       </c>
       <c r="D81">
         <v>2</v>
       </c>
       <c r="E81">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="F81">
-        <v>2.6019811630248999E-2</v>
-      </c>
-      <c r="G81">
-        <v>2.5000000000000001E-2</v>
+        <v>0.28670001029968201</v>
+      </c>
+      <c r="G81" s="4">
+        <v>9.375E-2</v>
       </c>
       <c r="H81">
-        <v>56512</v>
+        <v>178472</v>
       </c>
       <c r="I81">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="J81">
         <v>128</v>
@@ -3040,31 +3150,31 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
         <v>14</v>
       </c>
       <c r="C82">
-        <v>69</v>
+        <v>451</v>
       </c>
       <c r="D82">
         <v>2</v>
       </c>
       <c r="E82">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F82">
-        <v>3.5067558288574198E-2</v>
-      </c>
-      <c r="G82">
-        <v>7.9365079365079309E-3</v>
+        <v>0.55692172050475997</v>
+      </c>
+      <c r="G82" s="4">
+        <v>3.125E-2</v>
       </c>
       <c r="H82">
-        <v>88645</v>
+        <v>182768</v>
       </c>
       <c r="I82">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J82">
         <v>128</v>
@@ -3072,31 +3182,31 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B83" t="s">
         <v>14</v>
       </c>
       <c r="C83">
-        <v>93</v>
+        <v>559</v>
       </c>
       <c r="D83">
         <v>2</v>
       </c>
       <c r="E83">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="F83">
-        <v>5.2066802978515597E-2</v>
-      </c>
-      <c r="G83">
-        <v>5.5118110236220402E-2</v>
+        <v>0.84226179122924805</v>
+      </c>
+      <c r="G83" s="4">
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>87028</v>
+        <v>252281</v>
       </c>
       <c r="I83">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J83">
         <v>128</v>
@@ -3104,193 +3214,33 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B84" t="s">
         <v>14</v>
       </c>
       <c r="C84">
-        <v>119</v>
+        <v>699</v>
       </c>
       <c r="D84">
         <v>2</v>
       </c>
       <c r="E84">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="F84">
-        <v>7.6587200164794894E-2</v>
-      </c>
-      <c r="G84">
-        <v>3.125E-2</v>
+        <v>1.0255815982818599</v>
+      </c>
+      <c r="G84" s="4">
+        <v>0</v>
       </c>
       <c r="H84">
-        <v>88724</v>
+        <v>250903</v>
       </c>
       <c r="I84">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J84">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A85" t="s">
-        <v>52</v>
-      </c>
-      <c r="B85" t="s">
-        <v>14</v>
-      </c>
-      <c r="C85">
-        <v>203</v>
-      </c>
-      <c r="D85">
-        <v>2</v>
-      </c>
-      <c r="E85">
-        <v>31</v>
-      </c>
-      <c r="F85">
-        <v>0.21200394630432101</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>131034</v>
-      </c>
-      <c r="I85">
-        <v>34</v>
-      </c>
-      <c r="J85">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A86" t="s">
-        <v>52</v>
-      </c>
-      <c r="B86" t="s">
-        <v>14</v>
-      </c>
-      <c r="C86">
-        <v>341</v>
-      </c>
-      <c r="D86">
-        <v>2</v>
-      </c>
-      <c r="E86">
-        <v>47</v>
-      </c>
-      <c r="F86">
-        <v>0.28670001029968201</v>
-      </c>
-      <c r="G86">
-        <v>9.375E-2</v>
-      </c>
-      <c r="H86">
-        <v>178472</v>
-      </c>
-      <c r="I86">
-        <v>38</v>
-      </c>
-      <c r="J86">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A87" t="s">
-        <v>52</v>
-      </c>
-      <c r="B87" t="s">
-        <v>14</v>
-      </c>
-      <c r="C87">
-        <v>451</v>
-      </c>
-      <c r="D87">
-        <v>2</v>
-      </c>
-      <c r="E87">
-        <v>44</v>
-      </c>
-      <c r="F87">
-        <v>0.55692172050475997</v>
-      </c>
-      <c r="G87">
-        <v>3.125E-2</v>
-      </c>
-      <c r="H87">
-        <v>182768</v>
-      </c>
-      <c r="I87">
-        <v>38</v>
-      </c>
-      <c r="J87">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A88" t="s">
-        <v>52</v>
-      </c>
-      <c r="B88" t="s">
-        <v>14</v>
-      </c>
-      <c r="C88">
-        <v>559</v>
-      </c>
-      <c r="D88">
-        <v>2</v>
-      </c>
-      <c r="E88">
-        <v>57</v>
-      </c>
-      <c r="F88">
-        <v>0.84226179122924805</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>252281</v>
-      </c>
-      <c r="I88">
-        <v>42</v>
-      </c>
-      <c r="J88">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A89" t="s">
-        <v>52</v>
-      </c>
-      <c r="B89" t="s">
-        <v>14</v>
-      </c>
-      <c r="C89">
-        <v>699</v>
-      </c>
-      <c r="D89">
-        <v>2</v>
-      </c>
-      <c r="E89">
-        <v>60</v>
-      </c>
-      <c r="F89">
-        <v>1.0255815982818599</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>250903</v>
-      </c>
-      <c r="I89">
-        <v>42</v>
-      </c>
-      <c r="J89">
         <v>128</v>
       </c>
     </row>
@@ -3322,62 +3272,62 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="I2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="C3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="I3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3385,34 +3335,34 @@
       <c r="A5">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1">
         <v>9.5086097717285104E-3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>0.2734375</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>17275</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>18</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="2">
         <v>1.18474960327148E-2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="2">
         <v>1.0523796081542899E-2</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <v>0.27500000000000002</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <v>17275</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <v>18</v>
       </c>
     </row>
@@ -3420,646 +3370,646 @@
       <c r="A6">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1">
         <v>9.2699527740478498E-3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>0.16521739130434701</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>32912</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>22</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="2">
         <v>1.1539459228515601E-4</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="2">
         <v>9.5095634460449201E-3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <v>0.23728813559322001</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>32912</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <v>22</v>
       </c>
-      <c r="R6" s="6" t="s">
-        <v>58</v>
+      <c r="R6" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1">
         <v>1.85952186584472E-2</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>56384</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>26</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="2">
         <v>1.1467933654785099E-4</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="2">
         <v>3.70151996612548E-2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <v>56384</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <v>26</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>60</v>
+      <c r="R7" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>35</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1">
         <v>1.80227756500244E-2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>3.9370078740157403E-2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>56516</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>26</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="2">
         <v>1.3899803161620999E-4</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="2">
         <v>4.1440725326538003E-2</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <v>0.180722891566265</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <v>56516</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <v>26</v>
       </c>
-      <c r="R8" s="6" t="s">
-        <v>61</v>
+      <c r="R8" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>51</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1">
         <v>2.7544021606445299E-2</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>7.03125E-2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="1">
         <v>54973</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>26</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="2">
         <v>1.3446807861328101E-4</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="2">
         <v>1.6571044921875E-2</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <v>0.18333333333333299</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>54973</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <v>26</v>
       </c>
-      <c r="R9" s="6" t="s">
-        <v>62</v>
+      <c r="R9" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>55</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1">
         <v>2.6019811630248999E-2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>56512</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>26</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="2">
         <v>1.0776519775390601E-4</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="2">
         <v>4.9282550811767502E-2</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="2">
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="2">
         <v>56512</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="2">
         <v>26</v>
       </c>
-      <c r="R10" s="6" t="s">
-        <v>64</v>
+      <c r="R10" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>69</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1">
         <v>3.5067558288574198E-2</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>7.9365079365079309E-3</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>88645</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>30</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="R11" s="6" t="s">
-        <v>66</v>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="R11" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>93</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="1">
         <v>5.2066802978515597E-2</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>5.5118110236220402E-2</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>87028</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>30</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="R12" s="6" t="s">
-        <v>68</v>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="R12" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>119</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1">
         <v>7.6587200164794894E-2</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="1">
         <v>88724</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="1">
         <v>30</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="R13" s="6" t="s">
-        <v>66</v>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="R13" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>203</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.21200394630432101</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="1">
         <v>131034</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="1">
         <v>34</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="R14" s="6" t="s">
-        <v>71</v>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="R14" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>341</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1">
         <v>0.28670001029968201</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="1">
         <v>9.375E-2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="1">
         <v>178472</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="1">
         <v>38</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="R15" s="6" t="s">
-        <v>66</v>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="R15" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>451</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1">
         <v>0.55692172050475997</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="1">
         <v>182768</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="1">
         <v>38</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="R16" s="6" t="s">
-        <v>74</v>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="R16" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>559</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.84226179122924805</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="1">
         <v>252281</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="1">
         <v>42</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="R17" s="6" t="s">
-        <v>66</v>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="R17" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>699</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="1">
         <v>1.0255815982818599</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="1">
         <v>250903</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>42</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="R18" s="6" t="s">
-        <v>77</v>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="R18" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>815</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="R19" s="6" t="s">
-        <v>78</v>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="R19" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>943</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="R20" s="6" t="s">
-        <v>79</v>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="R20" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>1067</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="R21" s="6" t="s">
-        <v>78</v>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="R21" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>1167</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="R22" s="6" t="s">
-        <v>80</v>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="R22" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>1263</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="R23" s="6" t="s">
-        <v>78</v>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="R23" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>1363</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="R24" s="6" t="s">
-        <v>81</v>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="R24" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>1469</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="R25" s="6" t="s">
-        <v>82</v>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="R25" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>1589</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="R26" s="6" t="s">
-        <v>83</v>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="R26" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>1703</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="R27" s="6" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="R27" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="R28" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="R29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="R30" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="R31" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="R32" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="R28" s="6" t="s">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R33" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R34" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="R29" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="R30" s="6" t="s">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R35" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R36" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="R31" s="6" t="s">
+    <row r="37" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R37" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R38" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="R32" s="6" t="s">
+    <row r="39" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R39" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R33" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R34" s="6" t="s">
+    <row r="40" spans="18:18" x14ac:dyDescent="0.5">
+      <c r="R40" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R35" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R36" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R37" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R38" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R39" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R40" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="41" spans="18:18" x14ac:dyDescent="0.5">
-      <c r="R41" s="6" t="s">
-        <v>92</v>
+      <c r="R41" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>